<commit_message>
plan of phase 2
</commit_message>
<xml_diff>
--- a/程序员客栈项目/因卓科技教育平台/因卓教育阶段二/软件设计/前后端接口列表.xlsx
+++ b/程序员客栈项目/因卓科技教育平台/因卓教育阶段二/软件设计/前后端接口列表.xlsx
@@ -4,12 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="首页" sheetId="1" r:id="rId1"/>
     <sheet name="学情" sheetId="2" r:id="rId2"/>
     <sheet name="阅卷" sheetId="3" r:id="rId3"/>
+    <sheet name="其他" sheetId="4" r:id="rId4"/>
+    <sheet name="学校" sheetId="5" r:id="rId5"/>
+    <sheet name="题库" sheetId="6" r:id="rId6"/>
+    <sheet name="考试" sheetId="7" r:id="rId7"/>
+    <sheet name="推送" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="172">
   <si>
     <t>获取班级的简要学情信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1402,6 +1407,142 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>高级搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精确搜索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取评卷员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置评卷员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置评分模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取扫描仪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置图像存储目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取扫描信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WINDOWS服务实时推送扫描信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取扫描异常信息（包含准考证异常、准考证重复、答题卡图像不合格、客观题填涂异常、缺考答题卡信息）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取扫描纪录信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载扫描纪录信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交批改结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取小题信息（如果是已经批改的试题，返回批改结果）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学校管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>班级管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教师管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学生管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>考试类型配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结业升班管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学校套题库管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加考试类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑考试类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除考试类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升班</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加目录结构名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑目录结构名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除目录结构名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试题审核</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加试题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑试题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试题属性设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试题管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1421,6 +1562,132 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>_4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>开始扫描</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>阅卷管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>开始扫描</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>开始批改</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>阅卷管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>阅卷设置</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>阅卷管理</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>_1</t>
     </r>
     <r>
@@ -1437,181 +1704,229 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>高级搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精确搜索</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>阅卷管理</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>阅卷设置</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取评卷员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置评卷员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置评分模式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>阅卷管理</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>开始扫描</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取扫描仪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置图像存储目录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取扫描信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WINDOWS服务实时推送扫描信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取扫描异常信息（包含准考证异常、准考证重复、答题卡图像不合格、客观题填涂异常、缺考答题卡信息）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取扫描纪录信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>下载扫描纪录信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>阅卷管理</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>开始扫描</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>开始批改</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提交批改结果</t>
+    <t>获取试题列表
+     &gt; 可以根据知识点、章节点筛选
+     &gt; 根据不同数据项进行排序
+     &gt; 根据题干信息里面的关键字、题号查询试题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">获取试题列表
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">可以根据知识点、章节点筛选
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">根据不同数据项进行排序
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>根据题干信息里面的关键字、题号查询试题</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取试卷列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>智能组卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真题还原</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取真题试卷列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>题库浏览</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分享试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取分享的试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>试卷管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>考试列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取考试列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匹配试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看考试详情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载考试试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载考试答题卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布成绩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取扫描仪信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置本地图像存储目录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取答题卡切图区域信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>作业列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取作业列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匹配试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看作业详情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载作业试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载作业答题卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>套题列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取套题列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建套题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建考试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建作业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看套题详情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载套题试卷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下载套题答题卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推送</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发布消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撤回消息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看消息详情</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1663,22 +1978,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1963,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1975,7 +2293,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1983,31 +2301,31 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2018,31 +2336,31 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2050,13 +2368,13 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2064,13 +2382,13 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2078,31 +2396,31 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="3"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="3"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="3"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2124,19 +2442,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="22.69921875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.69921875" style="2" customWidth="1"/>
     <col min="2" max="2" width="46.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2144,37 +2462,37 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2182,31 +2500,31 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2214,19 +2532,19 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="5"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2234,31 +2552,31 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="5"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="5"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="5"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2272,61 +2590,61 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="5"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="5"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="5"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="5"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="5"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="5"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="5"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="5"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2340,61 +2658,61 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="5"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="5"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="5"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="5"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="5"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="5"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="5"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="5"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="5"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="5"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
@@ -2408,37 +2726,37 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="5"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="5"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="5"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="5"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="5"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="5"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="1" t="s">
         <v>39</v>
       </c>
@@ -2447,7 +2765,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="5"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="1" t="s">
         <v>40</v>
       </c>
@@ -2456,7 +2774,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="5"/>
+      <c r="A51" s="7"/>
       <c r="B51" s="1" t="s">
         <v>41</v>
       </c>
@@ -2465,13 +2783,13 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="5"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="5"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="1" t="s">
         <v>50</v>
       </c>
@@ -2485,61 +2803,61 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="5"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="5"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="5"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="5"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="5"/>
+      <c r="A59" s="7"/>
       <c r="B59" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="5"/>
+      <c r="A60" s="7"/>
       <c r="B60" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="5"/>
+      <c r="A61" s="7"/>
       <c r="B61" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="5"/>
+      <c r="A62" s="7"/>
       <c r="B62" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="5"/>
+      <c r="A63" s="7"/>
       <c r="B63" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="5"/>
+      <c r="A64" s="7"/>
       <c r="B64" s="1" t="s">
         <v>51</v>
       </c>
@@ -2553,19 +2871,19 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="5"/>
+      <c r="A66" s="7"/>
       <c r="B66" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="7"/>
       <c r="B67" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="5"/>
+      <c r="A68" s="7"/>
       <c r="B68" s="1" t="s">
         <v>58</v>
       </c>
@@ -2579,31 +2897,31 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="5"/>
+      <c r="A70" s="7"/>
       <c r="B70" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="5"/>
+      <c r="A71" s="7"/>
       <c r="B71" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="5"/>
+      <c r="A72" s="7"/>
       <c r="B72" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="5"/>
+      <c r="A73" s="7"/>
       <c r="B73" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="5"/>
+      <c r="A74" s="7"/>
       <c r="B74" s="1" t="s">
         <v>51</v>
       </c>
@@ -2617,7 +2935,7 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="5"/>
+      <c r="A76" s="7"/>
       <c r="B76" s="1" t="s">
         <v>57</v>
       </c>
@@ -2626,13 +2944,13 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="5"/>
+      <c r="A77" s="7"/>
       <c r="B77" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="5"/>
+      <c r="A78" s="7"/>
       <c r="B78" s="1" t="s">
         <v>61</v>
       </c>
@@ -2646,31 +2964,31 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="5"/>
+      <c r="A80" s="7"/>
       <c r="B80" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="5"/>
+      <c r="A81" s="7"/>
       <c r="B81" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="5"/>
+      <c r="A82" s="7"/>
       <c r="B82" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="5"/>
+      <c r="A83" s="7"/>
       <c r="B83" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="5"/>
+      <c r="A84" s="7"/>
       <c r="B84" s="1" t="s">
         <v>51</v>
       </c>
@@ -2684,19 +3002,19 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="5"/>
+      <c r="A86" s="7"/>
       <c r="B86" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="5"/>
+      <c r="A87" s="7"/>
       <c r="B87" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="5"/>
+      <c r="A88" s="7"/>
       <c r="B88" s="1" t="s">
         <v>66</v>
       </c>
@@ -2713,25 +3031,25 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="5"/>
+      <c r="A90" s="7"/>
       <c r="B90" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="5"/>
+      <c r="A91" s="7"/>
       <c r="B91" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="5"/>
+      <c r="A92" s="7"/>
       <c r="B92" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="5"/>
+      <c r="A93" s="7"/>
       <c r="B93" s="1" t="s">
         <v>69</v>
       </c>
@@ -2745,19 +3063,19 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="5"/>
+      <c r="A95" s="7"/>
       <c r="B95" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="5"/>
+      <c r="A96" s="7"/>
       <c r="B96" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:2">
-      <c r="A97" s="5"/>
+      <c r="A97" s="7"/>
       <c r="B97" s="1" t="s">
         <v>0</v>
       </c>
@@ -2771,115 +3089,115 @@
       </c>
     </row>
     <row r="99" spans="1:2">
-      <c r="A99" s="5"/>
+      <c r="A99" s="7"/>
       <c r="B99" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="100" spans="1:2">
-      <c r="A100" s="5"/>
+      <c r="A100" s="7"/>
       <c r="B100" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="5"/>
+      <c r="A101" s="7"/>
       <c r="B101" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="5"/>
+      <c r="A102" s="7"/>
       <c r="B102" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="103" spans="1:2">
-      <c r="A103" s="5"/>
+      <c r="A103" s="7"/>
       <c r="B103" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="104" spans="1:2">
-      <c r="A104" s="5"/>
+      <c r="A104" s="7"/>
       <c r="B104" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="105" spans="1:2">
-      <c r="A105" s="5"/>
+      <c r="A105" s="7"/>
       <c r="B105" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="5"/>
+      <c r="A106" s="7"/>
       <c r="B106" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="107" spans="1:2">
-      <c r="A107" s="5"/>
+      <c r="A107" s="7"/>
       <c r="B107" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="5"/>
+      <c r="A108" s="7"/>
       <c r="B108" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="A109" s="5"/>
+      <c r="A109" s="7"/>
       <c r="B109" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="110" spans="1:2">
-      <c r="A110" s="5"/>
+      <c r="A110" s="7"/>
       <c r="B110" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:2">
-      <c r="A111" s="5"/>
+      <c r="A111" s="7"/>
       <c r="B111" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="5"/>
+      <c r="A112" s="7"/>
       <c r="B112" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="5"/>
+      <c r="A113" s="7"/>
       <c r="B113" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="5"/>
+      <c r="A114" s="7"/>
       <c r="B114" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="5"/>
+      <c r="A115" s="7"/>
       <c r="B115" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="5"/>
+      <c r="A116" s="7"/>
       <c r="B116" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="5"/>
+      <c r="A117" s="7"/>
       <c r="B117" s="1" t="s">
         <v>90</v>
       </c>
@@ -2893,7 +3211,7 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="5"/>
+      <c r="A119" s="7"/>
       <c r="B119" s="1" t="s">
         <v>93</v>
       </c>
@@ -2902,43 +3220,49 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="5"/>
+      <c r="A120" s="7"/>
       <c r="B120" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="5"/>
+      <c r="A121" s="7"/>
       <c r="B121" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="5"/>
+      <c r="A122" s="7"/>
       <c r="B122" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="5"/>
+      <c r="A123" s="7"/>
       <c r="B123" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="5"/>
+      <c r="A124" s="7"/>
       <c r="B124" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="5"/>
+      <c r="A125" s="7"/>
       <c r="B125" s="1" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A32:A42"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A31"/>
     <mergeCell ref="A89:A93"/>
     <mergeCell ref="A94:A97"/>
     <mergeCell ref="A98:A117"/>
@@ -2950,12 +3274,6 @@
     <mergeCell ref="A54:A64"/>
     <mergeCell ref="A79:A84"/>
     <mergeCell ref="A85:A88"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A31"/>
-    <mergeCell ref="A32:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2965,10 +3283,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2978,80 +3296,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="B2" s="1" t="s">
-        <v>98</v>
+      <c r="A2" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="B4" s="1" t="s">
-        <v>101</v>
+      <c r="A4" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:2">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3059,4 +3506,314 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="59.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="55.2">
+      <c r="A7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="55.2">
+      <c r="A11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="22.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="B28" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>